<commit_message>
Changed a few graphs
</commit_message>
<xml_diff>
--- a/dummy_tests_results.xlsx
+++ b/dummy_tests_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\COMP\COMP551\Exploring_papers\COMP551_reproductibility_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9DEDB5-5F2C-4DF2-A261-B336371397D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9C7623-609E-4365-86AB-D2F8857ED441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="3" xr2:uid="{F901F0DE-0FAB-624D-80E6-457D668F2158}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{F901F0DE-0FAB-624D-80E6-457D668F2158}"/>
   </bookViews>
   <sheets>
     <sheet name="Training Time for Full Batch" sheetId="2" r:id="rId1"/>
@@ -464,121 +464,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>BNA+LO</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Full Batch'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Full Batch'!$J$3:$J$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>22.663358926773</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.029124379157999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.4277993440628</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.536662220954801</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.2021436691284</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16.691946387290901</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14.476787447929301</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16.021446228027301</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17.053970694541899</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.241069793701101</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6BE5-0743-BC56-600749F28062}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
@@ -1179,6 +1064,139 @@
         </c:dLbls>
         <c:axId val="2016617759"/>
         <c:axId val="2042978671"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>BNA+LO</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Full Batch'!$A$3:$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Full Batch'!$J$3:$J$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>22.663358926773</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16.029124379157999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>15.4277993440628</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>13.536662220954801</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>15.2021436691284</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>16.691946387290901</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>14.476787447929301</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>16.021446228027301</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>17.053970694541899</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>16.241069793701101</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-6BE5-0743-BC56-600749F28062}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="2016617759"/>
@@ -1781,121 +1799,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>BNA+LO</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Full Batch'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Full Batch'!$L$3:$L$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.38574999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.67015000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.71255000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.75085000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.75455000000000005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.76934999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.77574999999999905</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.76869999999999905</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.78644999999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.79330000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4295-6E47-B30D-C4941D4AC40F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
@@ -2496,6 +2399,139 @@
         </c:dLbls>
         <c:axId val="2016617759"/>
         <c:axId val="2042978671"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>BNA+LO</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Full Batch'!$A$3:$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Full Batch'!$L$3:$L$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>0.38574999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.67015000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.71255000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.75085000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.75455000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.76934999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.77574999999999905</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.76869999999999905</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.78644999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.79330000000000001</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-4295-6E47-B30D-C4941D4AC40F}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="2016617759"/>
@@ -3098,121 +3134,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>BNA+LO</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Full Batch'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'500 Batch'!$J$3:$J$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>7.8651769199999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.8572782300000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.5248359399999991</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.2468485</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.0702152</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.089029399999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.022588000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.9083589</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12.404959399999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13.3672348</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C921-954A-A1DB-2B34F9AB4765}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
@@ -3813,6 +3734,139 @@
         </c:dLbls>
         <c:axId val="2016617759"/>
         <c:axId val="2042978671"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>BNA+LO</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Full Batch'!$A$3:$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'500 Batch'!$J$3:$J$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>7.8651769199999997</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7.8572782300000004</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9.5248359399999991</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>10.2468485</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>10.0702152</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>11.089029399999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>13.022588000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>12.9083589</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>12.404959399999999</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>13.3672348</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-C921-954A-A1DB-2B34F9AB4765}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="2016617759"/>
@@ -4414,121 +4468,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>BNA+LO</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Full Batch'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'500 Batch'!$L$3:$L$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.42344999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.65669999999999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70540000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.74070000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.75129999999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.76839999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.77575000000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.77510000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.78349999999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.78580000000000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-825E-7F44-B94A-E916C4958AB2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
@@ -5129,6 +5068,139 @@
         </c:dLbls>
         <c:axId val="2016617759"/>
         <c:axId val="2042978671"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>BNA+LO</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Full Batch'!$A$3:$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'500 Batch'!$L$3:$L$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>0.42344999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.65669999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.70540000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.74070000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.75129999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.76839999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.77575000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.77510000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.78349999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.78580000000000005</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-825E-7F44-B94A-E916C4958AB2}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="2016617759"/>
@@ -7652,7 +7724,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6D4365B6-DE6B-3347-88AC-2F961170C945}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="176" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7685,7 +7757,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{8A95509C-D5E3-D341-85B9-A6F87908E5B3}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0"/>
+    <sheetView zoomScale="134" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8123,7 +8195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9208E61D-BEFE-6841-9EAE-8656453D96B6}">
   <dimension ref="A1:AK12"/>
   <sheetViews>
-    <sheetView topLeftCell="P15" workbookViewId="0">
+    <sheetView topLeftCell="P3" workbookViewId="0">
       <selection sqref="A1:AK12"/>
     </sheetView>
   </sheetViews>

</xml_diff>